<commit_message>
Tentativa de gerar novos resultados
</commit_message>
<xml_diff>
--- a/data/passwords.xlsx
+++ b/data/passwords.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>senha123</t>
+          <t>password</t>
         </is>
       </c>
     </row>
@@ -464,42 +464,679 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>P@ssw0rd2024</t>
+          <t>abc123</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Amigo2023</t>
+          <t>111111</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Casa2021!</t>
+          <t>123123</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tr3ndMUsic!99</t>
+          <t>senha123</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>G#7xF!m2Lq8</t>
+          <t>iloveyou</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>admin</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>welcome</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>monkey</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>letmein</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>football</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dragon</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>sunshine</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>master</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>hello</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>freedom</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>whatever</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>login</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>flower</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>shadow</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>princess</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>qazwsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>password1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Casa2021!</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Amigo2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Tr3ndMUsic!99</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Brasil2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Natura#21</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>P@ssw0rd2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Summer2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>C0ffeelover</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Joao#2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Mari_1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Senha@Forte</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>L0gin@2023</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>G@mingLife99</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Study#Mode</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BookLover22</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Work!Hard</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>TimeToCode</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>BeHappy24</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>P@raSempre</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SkyBlue77</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Star!Dust9</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>C@fezinho</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Strong#Mind</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Peace&amp;Love</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>MyDog123</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>OceanView!</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mountain#Top</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Tr@velNow</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>MyHeart22</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>GoodLuck!77</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Plan#2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Smart123</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Victory!</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Future@Goal</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>S@feHouse</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>R3li@bl3P@55w0rd!</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>G#7xF!m2Lq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>XyZ!93z@P1</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>N!ghtFalcon@2048</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>9pT@zR!4yU</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>W@terF0x#22</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>0mega#2025!</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>F!r3Str0m_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Z@pper_77!</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>P0w3rM!nd#1</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>T!tanium_S3c</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>R@inB0w#2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Cr!pt0K3y#</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>B@ckDoor99!</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>N3ural#Link@</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Qw3rTy#9087</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>S3cur3!Vault</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>M@trix#Reboot</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>H@shBuster99</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Quantum#AI!</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Infini#Loop@</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>D@taShield42</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Z#ph1r9L@b</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Cyb3rW@ll!</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Encrypt#Me9</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Deep#Sea2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>4rcT!cW0lf@</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>S@turnR!ng5</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>0verCl0ck#77</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>S!lverH@wk</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>H@ckPr00f!Key</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Mega#Core!99</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>5up3rS@fe#P@ss</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>P@thF!nderX</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Unbr3@k@ble#2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>B!oSecur3X!</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Neural#Web!</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>S@feZone#999</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Tru$tMe#42</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Bl@ckH0le#AI</t>
         </is>
       </c>
     </row>

</xml_diff>